<commit_message>
Added fig and doc in README; added topic in Excel file
</commit_message>
<xml_diff>
--- a/research-seminars.xlsx
+++ b/research-seminars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uio-my.sharepoint.com/personal/jacobjc_uio_no/Documents/research-seminars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="11_B25C5E92FC310840C84FF8F5B8BE080D877FEB4B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4039D45D-C827-4630-8322-B12D5CBD72DC}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_B25C5E92FC310840C84FF8F5B8BE080D877FEB4B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AA8306DD-371A-4B6F-B481-33E469BBC3AA}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="91">
   <si>
     <t>#</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>2020-03-23</t>
+  </si>
+  <si>
+    <t>Penalized regression: LASSO and ridge regression</t>
   </si>
 </sst>
 </file>
@@ -4874,11 +4877,11 @@
     <tabColor rgb="FF0000FF"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1005"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5141,7 +5144,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="E14" s="19"/>
     </row>
@@ -5156,7 +5159,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="19"/>
     </row>
@@ -5171,7 +5174,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" s="19"/>
     </row>
@@ -5186,7 +5189,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E17" s="19"/>
     </row>
@@ -5201,7 +5204,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E18" s="19"/>
     </row>
@@ -5216,7 +5219,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="19"/>
     </row>
@@ -5228,17 +5231,12 @@
         <v>20</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E20" s="19"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
@@ -5251,9 +5249,14 @@
         <v>34</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
@@ -5266,14 +5269,9 @@
         <v>34</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E22" s="19"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
@@ -5283,12 +5281,17 @@
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="19"/>
+        <v>37</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
@@ -5301,7 +5304,7 @@
         <v>38</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E24" s="19"/>
     </row>
@@ -5315,15 +5318,10 @@
       <c r="C25" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>85</v>
-      </c>
+      <c r="D25" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="19"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
@@ -5335,10 +5333,15 @@
       <c r="C26" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="19"/>
+      <c r="D26" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
@@ -5351,14 +5354,9 @@
         <v>38</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="20">
-        <v>43067</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>85</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E27" s="19"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
@@ -5371,10 +5369,10 @@
         <v>38</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E28" s="20">
-        <v>43111</v>
+        <v>43067</v>
       </c>
       <c r="F28" s="23" t="s">
         <v>85</v>
@@ -5391,9 +5389,14 @@
         <v>38</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="19"/>
+        <v>43</v>
+      </c>
+      <c r="E29" s="20">
+        <v>43111</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
@@ -5406,7 +5409,7 @@
         <v>38</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E30" s="19"/>
     </row>
@@ -5421,7 +5424,7 @@
         <v>38</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" s="19"/>
     </row>
@@ -5436,7 +5439,7 @@
         <v>38</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" s="19"/>
     </row>
@@ -5451,7 +5454,7 @@
         <v>38</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="19"/>
     </row>
@@ -5466,7 +5469,7 @@
         <v>38</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E34" s="19"/>
     </row>
@@ -5481,7 +5484,7 @@
         <v>38</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E35" s="19"/>
     </row>
@@ -5496,29 +5499,29 @@
         <v>38</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E37" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
@@ -5531,7 +5534,7 @@
         <v>54</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E38" s="19"/>
     </row>
@@ -5543,10 +5546,10 @@
         <v>53</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E39" s="19"/>
     </row>
@@ -5561,7 +5564,7 @@
         <v>34</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E40" s="19"/>
     </row>
@@ -5576,7 +5579,7 @@
         <v>34</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E41" s="19"/>
     </row>
@@ -5588,10 +5591,10 @@
         <v>53</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E42" s="19"/>
     </row>
@@ -5603,10 +5606,10 @@
         <v>53</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E43" s="19"/>
     </row>
@@ -5621,7 +5624,7 @@
         <v>67</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="19"/>
     </row>
@@ -5636,7 +5639,7 @@
         <v>67</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E45" s="19"/>
     </row>
@@ -5651,7 +5654,7 @@
         <v>67</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E46" s="19"/>
     </row>
@@ -5666,29 +5669,39 @@
         <v>67</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E47" s="19"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
+        <v>4</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="19"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="17">
         <v>5</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B49" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C49" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D49" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="20"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="17"/>
-      <c r="B49" s="21"/>
-      <c r="E49" s="19"/>
+      <c r="E49" s="20"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
@@ -10469,6 +10482,11 @@
       <c r="A1005" s="17"/>
       <c r="B1005" s="21"/>
       <c r="E1005" s="19"/>
+    </row>
+    <row r="1006" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1006" s="17"/>
+      <c r="B1006" s="21"/>
+      <c r="E1006" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added summary about LASSO/ridge
</commit_message>
<xml_diff>
--- a/research-seminars.xlsx
+++ b/research-seminars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uio-my.sharepoint.com/personal/jacobjc_uio_no/Documents/research-seminars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_B25C5E92FC310840C84FF8F5B8BE080D877FEB4B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AA8306DD-371A-4B6F-B481-33E469BBC3AA}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_B25C5E92FC310840C84FF8F5B8BE080D877FEB4B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8857C181-F6BC-4D1D-92E6-C4BA4712FA93}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="104">
   <si>
     <t>#</t>
   </si>
@@ -295,6 +295,45 @@
   <si>
     <t>Penalized regression: LASSO and ridge regression</t>
   </si>
+  <si>
+    <t>2020-03-30</t>
+  </si>
+  <si>
+    <t>Amanda/Jacob</t>
+  </si>
+  <si>
+    <t>2020-04-06</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: data import (tidyr and friends)</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: data transformation (dplyr)</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: Rmarkdown</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: data visualization (ggplot2)</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: factors (forcats)</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: strings (stringr)</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: dates and times (lubridate)</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: apply functions (purrr)</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: RStudio IDE</t>
+  </si>
+  <si>
+    <t>RStudio cheatsheets: tidy evaluation (rlang)</t>
+  </si>
 </sst>
 </file>
 
@@ -386,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -448,6 +487,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4877,11 +4919,11 @@
     <tabColor rgb="FF0000FF"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1006"/>
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5146,7 +5188,12 @@
       <c r="D14" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="19"/>
+      <c r="E14" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
@@ -5159,9 +5206,12 @@
         <v>21</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="19"/>
+        <v>94</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
@@ -5174,9 +5224,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="19"/>
+        <v>95</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
@@ -5189,9 +5240,10 @@
         <v>21</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="19"/>
+        <v>97</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="18"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
@@ -5204,9 +5256,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="19"/>
+        <v>98</v>
+      </c>
+      <c r="E18" s="25"/>
+      <c r="F18" s="18"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
@@ -5219,9 +5272,10 @@
         <v>21</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
@@ -5234,9 +5288,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="19"/>
+        <v>100</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
@@ -5246,17 +5301,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
@@ -5266,12 +5317,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="19"/>
+        <v>96</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
@@ -5281,17 +5333,13 @@
         <v>20</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E23" s="25"/>
+      <c r="F23" s="18"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
@@ -5301,12 +5349,13 @@
         <v>20</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="19"/>
+        <v>103</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="F24" s="18"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="17">
@@ -5316,10 +5365,10 @@
         <v>20</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E25" s="19"/>
     </row>
@@ -5331,17 +5380,12 @@
         <v>20</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>85</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E26" s="19"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
@@ -5351,10 +5395,10 @@
         <v>20</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E27" s="19"/>
     </row>
@@ -5366,17 +5410,12 @@
         <v>20</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="20">
-        <v>43067</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>85</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E28" s="19"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
@@ -5386,17 +5425,12 @@
         <v>20</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="20">
-        <v>43111</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>85</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E29" s="19"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
@@ -5406,10 +5440,10 @@
         <v>20</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="E30" s="19"/>
     </row>
@@ -5421,12 +5455,17 @@
         <v>20</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="17">
@@ -5436,10 +5475,10 @@
         <v>20</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E32" s="19"/>
     </row>
@@ -5451,12 +5490,17 @@
         <v>20</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="19"/>
+        <v>37</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
@@ -5469,7 +5513,7 @@
         <v>38</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="E34" s="19"/>
     </row>
@@ -5484,7 +5528,7 @@
         <v>38</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E35" s="19"/>
     </row>
@@ -5498,10 +5542,15 @@
       <c r="C36" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E36" s="19"/>
+      <c r="D36" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
@@ -5514,164 +5563,174 @@
         <v>38</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F37" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="E37" s="19"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C38" s="18" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="19"/>
+        <v>42</v>
+      </c>
+      <c r="E38" s="20">
+        <v>43067</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="19"/>
+        <v>43</v>
+      </c>
+      <c r="E39" s="20">
+        <v>43111</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="E40" s="19"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E41" s="19"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="E42" s="19"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="E43" s="19"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="E44" s="19"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E45" s="19"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="E46" s="19"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E47" s="19"/>
+        <v>52</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
@@ -5681,77 +5740,177 @@
         <v>53</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="E48" s="19"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
+        <v>4</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" s="19"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="17">
+        <v>4</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E50" s="19"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
+        <v>4</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E51" s="19"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="17">
+        <v>4</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="19"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="17">
+        <v>4</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" s="19"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="17">
+        <v>4</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E54" s="19"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="17">
+        <v>4</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" s="19"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
+        <v>4</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E56" s="19"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="17">
+        <v>4</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" s="19"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="17">
+        <v>4</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E58" s="19"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
         <v>5</v>
       </c>
-      <c r="B49" s="18" t="s">
+      <c r="B59" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C59" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D59" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="20"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="17"/>
-      <c r="B50" s="21"/>
-      <c r="E50" s="19"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="17"/>
-      <c r="B51" s="21"/>
-      <c r="E51" s="19"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="B52" s="21"/>
-      <c r="E52" s="19"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="21"/>
-      <c r="E53" s="19"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="17"/>
-      <c r="B54" s="21"/>
-      <c r="E54" s="19"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="21"/>
-      <c r="E55" s="19"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="17"/>
-      <c r="B56" s="21"/>
-      <c r="E56" s="19"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="17"/>
-      <c r="B57" s="21"/>
-      <c r="E57" s="19"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="17"/>
-      <c r="B58" s="21"/>
-      <c r="E58" s="19"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="17"/>
-      <c r="B59" s="21"/>
-      <c r="E59" s="19"/>
+      <c r="E59" s="20"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="17"/>
@@ -10487,6 +10646,56 @@
       <c r="A1006" s="17"/>
       <c r="B1006" s="21"/>
       <c r="E1006" s="19"/>
+    </row>
+    <row r="1007" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1007" s="17"/>
+      <c r="B1007" s="21"/>
+      <c r="E1007" s="19"/>
+    </row>
+    <row r="1008" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1008" s="17"/>
+      <c r="B1008" s="21"/>
+      <c r="E1008" s="19"/>
+    </row>
+    <row r="1009" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1009" s="17"/>
+      <c r="B1009" s="21"/>
+      <c r="E1009" s="19"/>
+    </row>
+    <row r="1010" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1010" s="17"/>
+      <c r="B1010" s="21"/>
+      <c r="E1010" s="19"/>
+    </row>
+    <row r="1011" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1011" s="17"/>
+      <c r="B1011" s="21"/>
+      <c r="E1011" s="19"/>
+    </row>
+    <row r="1012" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1012" s="17"/>
+      <c r="B1012" s="21"/>
+      <c r="E1012" s="19"/>
+    </row>
+    <row r="1013" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1013" s="17"/>
+      <c r="B1013" s="21"/>
+      <c r="E1013" s="19"/>
+    </row>
+    <row r="1014" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1014" s="17"/>
+      <c r="B1014" s="21"/>
+      <c r="E1014" s="19"/>
+    </row>
+    <row r="1015" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1015" s="17"/>
+      <c r="B1015" s="21"/>
+      <c r="E1015" s="19"/>
+    </row>
+    <row r="1016" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1016" s="17"/>
+      <c r="B1016" s="21"/>
+      <c r="E1016" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tidytuesday week 20 - volcanos
</commit_message>
<xml_diff>
--- a/research-seminars.xlsx
+++ b/research-seminars.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uio-my.sharepoint.com/personal/jacobjc_uio_no/Documents/research-seminars/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_B25C5E92FC310840C84FF8F5B8BE080D877FEB4B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{10E75CE0-18AE-4884-A396-81B7619ECCEB}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="11_B25C5E92FC310840C84FF8F5B8BE080D877FEB4B" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{92816441-5F91-45C8-8CCA-07AEB646F855}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="115">
   <si>
     <t>#</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>See .Rmd file</t>
+  </si>
+  <si>
+    <t>2020-05-12</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Tidytuesday analysis</t>
+  </si>
+  <si>
+    <t>How to do peer review</t>
+  </si>
+  <si>
+    <t>2020-05-19</t>
   </si>
 </sst>
 </file>
@@ -449,7 +464,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -517,6 +532,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4944,11 +4962,11 @@
     <tabColor rgb="FF0000FF"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5503,16 +5521,19 @@
         <v>20</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>87</v>
+        <v>112</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -5526,9 +5547,14 @@
         <v>34</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
@@ -5541,14 +5567,9 @@
         <v>34</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E33" s="19"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
@@ -5558,12 +5579,17 @@
         <v>20</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="19"/>
+        <v>37</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
@@ -5576,7 +5602,7 @@
         <v>38</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E35" s="19"/>
     </row>
@@ -5590,15 +5616,10 @@
       <c r="C36" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>85</v>
-      </c>
+      <c r="D36" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
@@ -5610,12 +5631,14 @@
       <c r="C37" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="19"/>
-      <c r="H37" s="26" t="s">
-        <v>106</v>
+      <c r="D37" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -5629,13 +5652,11 @@
         <v>38</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" s="20">
-        <v>43067</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>85</v>
+        <v>41</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="H38" s="26" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -5649,10 +5670,10 @@
         <v>38</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E39" s="20">
-        <v>43111</v>
+        <v>43067</v>
       </c>
       <c r="F39" s="23" t="s">
         <v>85</v>
@@ -5669,9 +5690,14 @@
         <v>38</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="19"/>
+        <v>43</v>
+      </c>
+      <c r="E40" s="20">
+        <v>43111</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
@@ -5684,7 +5710,7 @@
         <v>38</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E41" s="19"/>
     </row>
@@ -5699,7 +5725,7 @@
         <v>38</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E42" s="19"/>
     </row>
@@ -5714,7 +5740,7 @@
         <v>38</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43" s="19"/>
     </row>
@@ -5729,7 +5755,7 @@
         <v>38</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E44" s="19"/>
     </row>
@@ -5744,7 +5770,7 @@
         <v>38</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E45" s="19"/>
     </row>
@@ -5759,7 +5785,7 @@
         <v>38</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E46" s="19"/>
     </row>
@@ -5774,31 +5800,31 @@
         <v>38</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F47" s="23" t="s">
-        <v>87</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="E47" s="19"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="19"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>4</v>
       </c>
@@ -5809,11 +5835,11 @@
         <v>54</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E49" s="19"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>4</v>
       </c>
@@ -5821,14 +5847,14 @@
         <v>53</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E50" s="19"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>4</v>
       </c>
@@ -5839,11 +5865,11 @@
         <v>34</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E51" s="19"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>4</v>
       </c>
@@ -5854,11 +5880,11 @@
         <v>34</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E52" s="19"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="17">
         <v>4</v>
       </c>
@@ -5866,14 +5892,14 @@
         <v>53</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E53" s="19"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="17">
         <v>4</v>
       </c>
@@ -5881,14 +5907,14 @@
         <v>53</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E54" s="19"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="17">
         <v>4</v>
       </c>
@@ -5899,11 +5925,11 @@
         <v>67</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E55" s="19"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="17">
         <v>4</v>
       </c>
@@ -5914,11 +5940,11 @@
         <v>67</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E56" s="19"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="17">
         <v>4</v>
       </c>
@@ -5929,11 +5955,11 @@
         <v>67</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E57" s="19"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>4</v>
       </c>
@@ -5944,46 +5970,71 @@
         <v>67</v>
       </c>
       <c r="D58" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E58" s="19"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
+        <v>4</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="17">
+        <v>4</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D60" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="E58" s="19"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
+      <c r="E60" s="19"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="17">
         <v>5</v>
       </c>
-      <c r="B59" s="18" t="s">
+      <c r="B61" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C59" s="18" t="s">
+      <c r="C61" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D59" s="18" t="s">
+      <c r="D61" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E59" s="20"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="17"/>
-      <c r="B60" s="21"/>
-      <c r="E60" s="19"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="17"/>
-      <c r="B61" s="21"/>
-      <c r="E61" s="19"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="20"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="17"/>
       <c r="B62" s="21"/>
       <c r="E62" s="19"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="17"/>
       <c r="B63" s="21"/>
       <c r="E63" s="19"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="17"/>
       <c r="B64" s="21"/>
       <c r="E64" s="19"/>
@@ -10747,6 +10798,16 @@
       <c r="A1016" s="17"/>
       <c r="B1016" s="21"/>
       <c r="E1016" s="19"/>
+    </row>
+    <row r="1017" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1017" s="17"/>
+      <c r="B1017" s="21"/>
+      <c r="E1017" s="19"/>
+    </row>
+    <row r="1018" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1018" s="17"/>
+      <c r="B1018" s="21"/>
+      <c r="E1018" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>